<commit_message>
Found parts for missing passives and added LiPo Battery
</commit_message>
<xml_diff>
--- a/Hardware/mood-badge-BOM.xlsx
+++ b/Hardware/mood-badge-BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\redne\Documents\Git\mood-badge-workshop\Hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73F9524-B928-43C1-BE90-01B60BF35655}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64B82D60-5733-4E61-AE2E-C8D1C7E692AC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1110" yWindow="1125" windowWidth="25875" windowHeight="13455" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="13455" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -235,7 +235,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F38" authorId="1" shapeId="0" xr:uid="{F49B0330-8D01-44C2-A6F4-DFE88908CC5C}">
+    <comment ref="F39" authorId="1" shapeId="0" xr:uid="{F49B0330-8D01-44C2-A6F4-DFE88908CC5C}">
       <text>
         <r>
           <rPr>
@@ -254,7 +254,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="239">
   <si>
     <t>BOM #</t>
   </si>
@@ -854,6 +854,123 @@
   </si>
   <si>
     <t>D1, D2, D3, D4, D5</t>
+  </si>
+  <si>
+    <t>ICSP</t>
+  </si>
+  <si>
+    <t>Unshielded Multilayer Inductor 300mOhm Max 0603 (1608 Metric) -</t>
+  </si>
+  <si>
+    <t>Taiyo Yuden</t>
+  </si>
+  <si>
+    <t>CKP1608D2R2M-T</t>
+  </si>
+  <si>
+    <t>587-6300-1-ND</t>
+  </si>
+  <si>
+    <t>210 ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RMCF0603FT210K</t>
+  </si>
+  <si>
+    <t>RMCF0603FT210KCT-ND</t>
+  </si>
+  <si>
+    <t>750 ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RMCF0603FT750K</t>
+  </si>
+  <si>
+    <t>RMCF0603FT750KCT-ND</t>
+  </si>
+  <si>
+    <t>487 ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>RC0603FR-07487RL</t>
+  </si>
+  <si>
+    <t>311-487HRCT-ND</t>
+  </si>
+  <si>
+    <t>180 ±1% 0.125W, 1/8W Chip Resistor 0603 (1608 Metric) Anti-Sulfur, Moisture Resistant Thin Film</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD180R</t>
+  </si>
+  <si>
+    <t>RNCP0603FTD180RCT-ND</t>
+  </si>
+  <si>
+    <t>12 ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RMCF0603FT12K0</t>
+  </si>
+  <si>
+    <t>RMCF0603FT12K0CT-ND</t>
+  </si>
+  <si>
+    <t>3.3 ±1% 0.1W, 1/10W Chip Resistor 0603 (1608 Metric) Automotive AEC-Q200 Thick Film</t>
+  </si>
+  <si>
+    <t>RMCF0603FT3M30</t>
+  </si>
+  <si>
+    <t>RMCF0603FT3M30CT-ND</t>
+  </si>
+  <si>
+    <t>±10% 6.3V Ceramic Capacitor X5R 0603 (1608 Metric)</t>
+  </si>
+  <si>
+    <t>CL10A475KQ8NNWC</t>
+  </si>
+  <si>
+    <t>1276-1902-1-ND</t>
+  </si>
+  <si>
+    <t>CAP CER 2.2PF 50V C0G/NP0 0603</t>
+  </si>
+  <si>
+    <t>CML0603C0G2R2CT50V</t>
+  </si>
+  <si>
+    <t>738-CML0603C0G2R2CT50VCT-ND</t>
+  </si>
+  <si>
+    <t>±20% 6.3V Ceramic Capacitor X5R 1206 (3216 Metric)</t>
+  </si>
+  <si>
+    <t>Murata Electronics</t>
+  </si>
+  <si>
+    <t>GRM31CR60J227ME11L</t>
+  </si>
+  <si>
+    <t>490-13970-1-ND</t>
+  </si>
+  <si>
+    <t>3.7v LiPo Battery</t>
+  </si>
+  <si>
+    <t>Lithium Ion Battery - 3.7v 2000mAh</t>
+  </si>
+  <si>
+    <t>JST</t>
+  </si>
+  <si>
+    <t>PKCELL</t>
+  </si>
+  <si>
+    <t>Adafruit</t>
+  </si>
+  <si>
+    <t>2011</t>
   </si>
 </sst>
 </file>
@@ -864,7 +981,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
   </numFmts>
-  <fonts count="14" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -954,15 +1071,8 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -978,12 +1088,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1179,8 +1283,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1190,6 +1292,8 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="4" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="83">
     <cellStyle name="Currency" xfId="82" builtinId="4"/>
@@ -1611,10 +1715,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O40"/>
+  <dimension ref="A1:O41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1637,12 +1741,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" s="3" customFormat="1" ht="14.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="24"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="22"/>
       <c r="E1" s="4"/>
       <c r="F1" s="15"/>
       <c r="G1" s="4"/>
@@ -1654,14 +1758,14 @@
         <v>11</v>
       </c>
       <c r="M1" s="6">
-        <f>SUM(M3:M75)</f>
-        <v>43.839999999999996</v>
+        <f>SUM(M3:M76)</f>
+        <v>59.42</v>
       </c>
       <c r="N1" s="12" t="s">
         <v>22</v>
       </c>
       <c r="O1" s="6">
-        <f>SUM(O3:O75)</f>
+        <f>SUM(O3:O76)</f>
         <v>0</v>
       </c>
     </row>
@@ -1750,7 +1854,7 @@
         <v>1</v>
       </c>
       <c r="M3" s="8">
-        <f t="shared" ref="M3:M38" si="0">K3*L3</f>
+        <f t="shared" ref="M3:M39" si="0">K3*L3</f>
         <v>2.14</v>
       </c>
       <c r="N3" s="10"/>
@@ -1848,6 +1952,9 @@
       <c r="B6" s="1" t="s">
         <v>194</v>
       </c>
+      <c r="C6" s="1" t="s">
+        <v>200</v>
+      </c>
       <c r="D6" s="1" t="s">
         <v>195</v>
       </c>
@@ -2101,38 +2208,32 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>87</v>
+        <v>233</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>88</v>
+        <v>234</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>89</v>
+        <v>235</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>90</v>
+        <v>236</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J12" s="1" t="s">
-        <v>92</v>
+        <v>237</v>
+      </c>
+      <c r="J12" s="24" t="s">
+        <v>238</v>
       </c>
       <c r="K12" s="10">
-        <v>0.95</v>
+        <v>12.5</v>
       </c>
       <c r="L12" s="1">
         <v>1</v>
       </c>
       <c r="M12" s="8">
         <f t="shared" si="0"/>
-        <v>0.95</v>
+        <v>12.5</v>
       </c>
       <c r="N12" s="10"/>
       <c r="O12" s="8"/>
@@ -2142,41 +2243,38 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>87</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>37</v>
+        <v>88</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>7</v>
+        <v>91</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>41</v>
+        <v>92</v>
       </c>
       <c r="K13" s="10">
-        <v>0.56000000000000005</v>
+        <v>0.95</v>
       </c>
       <c r="L13" s="1">
         <v>1</v>
       </c>
       <c r="M13" s="8">
         <f t="shared" si="0"/>
-        <v>0.56000000000000005</v>
+        <v>0.95</v>
       </c>
       <c r="N13" s="10"/>
       <c r="O13" s="8"/>
@@ -2186,41 +2284,41 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="K14" s="10">
-        <v>1.05</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="L14" s="1">
         <v>1</v>
       </c>
       <c r="M14" s="8">
         <f t="shared" si="0"/>
-        <v>1.05</v>
+        <v>0.56000000000000005</v>
       </c>
       <c r="N14" s="10"/>
       <c r="O14" s="8"/>
@@ -2230,41 +2328,41 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>49</v>
+        <v>10</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>163</v>
+        <v>31</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="I15" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>46</v>
+        <v>34</v>
       </c>
       <c r="K15" s="10">
-        <v>25.95</v>
+        <v>1.05</v>
       </c>
       <c r="L15" s="1">
         <v>1</v>
       </c>
       <c r="M15" s="8">
         <f t="shared" si="0"/>
-        <v>25.95</v>
+        <v>1.05</v>
       </c>
       <c r="N15" s="10"/>
       <c r="O15" s="8"/>
@@ -2274,83 +2372,85 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>21</v>
+        <v>48</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>73</v>
+        <v>43</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>38</v>
+        <v>163</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
       <c r="I16" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="K16" s="10">
-        <v>0.28999999999999998</v>
+        <v>25.95</v>
       </c>
       <c r="L16" s="1">
         <v>1</v>
       </c>
       <c r="M16" s="8">
         <f t="shared" si="0"/>
-        <v>0.28999999999999998</v>
-      </c>
+        <v>25.95</v>
+      </c>
+      <c r="N16" s="10"/>
+      <c r="O16" s="8"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>81</v>
+        <v>21</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>77</v>
+        <v>38</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>78</v>
+        <v>39</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="K17" s="10">
-        <v>1.04</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="L17" s="1">
         <v>1</v>
       </c>
       <c r="M17" s="8">
         <f t="shared" si="0"/>
-        <v>1.04</v>
+        <v>0.28999999999999998</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
@@ -2358,86 +2458,85 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>161</v>
+        <v>75</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="D18" s="19" t="s">
-        <v>189</v>
+        <v>81</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>76</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>190</v>
+        <v>77</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>191</v>
+        <v>78</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>192</v>
+        <v>79</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>193</v>
+        <v>80</v>
       </c>
       <c r="K18" s="10">
-        <v>1.05</v>
+        <v>1.04</v>
       </c>
       <c r="L18" s="1">
         <v>1</v>
       </c>
       <c r="M18" s="8">
-        <f>K18*L18</f>
-        <v>1.05</v>
-      </c>
-      <c r="N18" s="10"/>
-      <c r="O18" s="8"/>
+        <f t="shared" si="0"/>
+        <v>1.04</v>
+      </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>66</v>
+        <v>161</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>199</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>67</v>
+        <v>162</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>189</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F19" s="17" t="s">
-        <v>68</v>
+        <v>190</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>69</v>
+        <v>191</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>70</v>
+        <v>192</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>71</v>
+        <v>193</v>
       </c>
       <c r="K19" s="10">
-        <v>0.26</v>
+        <v>1.05</v>
       </c>
       <c r="L19" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="M19" s="8">
-        <f t="shared" si="0"/>
-        <v>1.3</v>
-      </c>
+        <f>K19*L19</f>
+        <v>1.05</v>
+      </c>
+      <c r="N19" s="10"/>
       <c r="O19" s="8"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
@@ -2445,43 +2544,42 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>117</v>
+        <v>66</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>122</v>
+        <v>199</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>118</v>
+        <v>67</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F20" s="18" t="s">
-        <v>13</v>
+      <c r="F20" s="17" t="s">
+        <v>68</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="I20" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>121</v>
+        <v>71</v>
       </c>
       <c r="K20" s="10">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
       <c r="L20" s="1">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="M20" s="8">
-        <f>K20*L20</f>
-        <v>2.7</v>
-      </c>
-      <c r="N20" s="10"/>
+        <f t="shared" si="0"/>
+        <v>1.3</v>
+      </c>
       <c r="O20" s="8"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
@@ -2489,25 +2587,41 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>149</v>
+        <v>117</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D21" s="21"/>
+        <v>122</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="E21" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K21" s="10"/>
+      <c r="G21" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="K21" s="10">
+        <v>0.27</v>
+      </c>
       <c r="L21" s="1">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M21" s="8">
         <f>K21*L21</f>
-        <v>0</v>
+        <v>2.7</v>
       </c>
       <c r="N21" s="10"/>
       <c r="O21" s="8"/>
@@ -2517,13 +2631,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>23</v>
+        <v>129</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>201</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>10</v>
@@ -2532,40 +2646,42 @@
         <v>13</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>15</v>
+        <v>202</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>24</v>
+        <v>203</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J22" s="1" t="s">
-        <v>25</v>
+        <v>204</v>
       </c>
       <c r="K22" s="10">
-        <v>0.01</v>
+        <v>0.16</v>
       </c>
       <c r="L22" s="1">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="M22" s="8">
-        <f t="shared" si="0"/>
-        <v>0.09</v>
-      </c>
+        <f>K22*L22</f>
+        <v>0.16</v>
+      </c>
+      <c r="N22" s="10"/>
+      <c r="O22" s="8"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
         <v>21</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>179</v>
+        <v>23</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>10</v>
@@ -2577,23 +2693,23 @@
         <v>15</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>180</v>
+        <v>24</v>
       </c>
       <c r="I23" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J23" s="1" t="s">
-        <v>181</v>
+        <v>25</v>
       </c>
       <c r="K23" s="10">
         <v>0.01</v>
       </c>
       <c r="L23" s="1">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="M23" s="8">
         <f t="shared" si="0"/>
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.2">
@@ -2601,13 +2717,13 @@
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>10</v>
@@ -2619,23 +2735,23 @@
         <v>15</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>172</v>
+        <v>180</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J24" s="1" t="s">
-        <v>173</v>
+        <v>181</v>
       </c>
       <c r="K24" s="10">
         <v>0.01</v>
       </c>
       <c r="L24" s="1">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="M24" s="8">
         <f t="shared" si="0"/>
-        <v>0.08</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.2">
@@ -2643,25 +2759,41 @@
         <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D25" s="20"/>
+        <v>135</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>171</v>
+      </c>
       <c r="E25" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K25" s="10"/>
+      <c r="G25" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="K25" s="10">
+        <v>0.01</v>
+      </c>
       <c r="L25" s="1">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="M25" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.2">
@@ -2669,25 +2801,41 @@
         <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="D26" s="20"/>
+        <v>137</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>205</v>
+      </c>
       <c r="E26" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F26" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K26" s="10"/>
+      <c r="G26" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="I26" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J26" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="K26" s="10">
+        <v>0.1</v>
+      </c>
       <c r="L26" s="1">
         <v>2</v>
       </c>
       <c r="M26" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.2">
@@ -2695,25 +2843,41 @@
         <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>141</v>
-      </c>
-      <c r="D27" s="20"/>
+        <v>139</v>
+      </c>
+      <c r="D27" s="19" t="s">
+        <v>208</v>
+      </c>
       <c r="E27" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F27" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K27" s="10"/>
+      <c r="G27" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="K27" s="10">
+        <v>0.1</v>
+      </c>
       <c r="L27" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M27" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.2">
@@ -2721,25 +2885,41 @@
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="D28" s="20"/>
+        <v>141</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>211</v>
+      </c>
       <c r="E28" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F28" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K28" s="10"/>
+      <c r="G28" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="K28" s="10">
+        <v>0.1</v>
+      </c>
       <c r="L28" s="1">
         <v>1</v>
       </c>
       <c r="M28" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.2">
@@ -2747,25 +2927,41 @@
         <v>27</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="D29" s="20"/>
+        <v>143</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>214</v>
+      </c>
       <c r="E29" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K29" s="10"/>
+      <c r="G29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="K29" s="10">
+        <v>0.1</v>
+      </c>
       <c r="L29" s="1">
         <v>1</v>
       </c>
       <c r="M29" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.2">
@@ -2773,13 +2969,13 @@
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>174</v>
+        <v>144</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>176</v>
+        <v>145</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>217</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>10</v>
@@ -2791,43 +2987,65 @@
         <v>15</v>
       </c>
       <c r="H30" s="1" t="s">
-        <v>177</v>
+        <v>218</v>
       </c>
       <c r="I30" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>178</v>
+        <v>219</v>
       </c>
       <c r="K30" s="10">
-        <v>0.01</v>
-      </c>
-      <c r="M30" s="8"/>
+        <v>0.1</v>
+      </c>
+      <c r="L30" s="1">
+        <v>1</v>
+      </c>
+      <c r="M30" s="8">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
         <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D31" s="20"/>
+        <v>175</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>176</v>
+      </c>
       <c r="E31" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K31" s="10"/>
+      <c r="G31" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="K31" s="10">
+        <v>0.01</v>
+      </c>
       <c r="L31" s="1">
         <v>1</v>
       </c>
       <c r="M31" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.2">
@@ -2835,13 +3053,13 @@
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>160</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>182</v>
+        <v>147</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>220</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>10</v>
@@ -2850,26 +3068,26 @@
         <v>13</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>183</v>
+        <v>15</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>184</v>
+        <v>221</v>
       </c>
       <c r="I32" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J32" s="1" t="s">
-        <v>185</v>
+        <v>222</v>
       </c>
       <c r="K32" s="10">
-        <v>0.03</v>
+        <v>0.1</v>
       </c>
       <c r="L32" s="1">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="M32" s="8">
         <f t="shared" si="0"/>
-        <v>0.3</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
@@ -2877,25 +3095,41 @@
         <v>31</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D33" s="20"/>
+        <v>160</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>182</v>
+      </c>
       <c r="E33" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K33" s="10"/>
+      <c r="G33" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="K33" s="10">
+        <v>0.03</v>
+      </c>
       <c r="L33" s="1">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="M33" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
@@ -2903,13 +3137,13 @@
         <v>32</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>186</v>
+        <v>151</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>223</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>10</v>
@@ -2921,23 +3155,23 @@
         <v>14</v>
       </c>
       <c r="H34" s="1" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="I34" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
       <c r="K34" s="10">
-        <v>7.0000000000000007E-2</v>
+        <v>0.1</v>
       </c>
       <c r="L34" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="M34" s="8">
         <f t="shared" si="0"/>
-        <v>0.21000000000000002</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -2945,25 +3179,41 @@
         <v>33</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D35" s="20"/>
+        <v>153</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>186</v>
+      </c>
       <c r="E35" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="10"/>
+      <c r="G35" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="K35" s="10">
+        <v>7.0000000000000007E-2</v>
+      </c>
       <c r="L35" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M35" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.21000000000000002</v>
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.2">
@@ -2971,13 +3221,13 @@
         <v>34</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>167</v>
+        <v>155</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>226</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>10</v>
@@ -2986,26 +3236,26 @@
         <v>13</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>168</v>
+        <v>15</v>
       </c>
       <c r="H36" s="1" t="s">
-        <v>169</v>
+        <v>227</v>
       </c>
       <c r="I36" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>170</v>
+        <v>228</v>
       </c>
       <c r="K36" s="10">
-        <v>0.13</v>
+        <v>0.1</v>
       </c>
       <c r="L36" s="1">
         <v>2</v>
       </c>
       <c r="M36" s="8">
         <f t="shared" si="0"/>
-        <v>0.26</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.2">
@@ -3013,13 +3263,13 @@
         <v>35</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>16</v>
+        <v>167</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>10</v>
@@ -3028,26 +3278,26 @@
         <v>13</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>14</v>
+        <v>168</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>17</v>
+        <v>169</v>
       </c>
       <c r="I37" s="1" t="s">
         <v>7</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>18</v>
+        <v>170</v>
       </c>
       <c r="K37" s="10">
-        <v>0.1</v>
+        <v>0.13</v>
       </c>
       <c r="L37" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M37" s="8">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
@@ -3055,32 +3305,90 @@
         <v>36</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D38" s="20"/>
+        <v>159</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="E38" s="1" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="K38" s="10"/>
+        <v>13</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="K38" s="10">
+        <v>0.1</v>
+      </c>
       <c r="L38" s="1">
         <v>1</v>
       </c>
       <c r="M38" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K39" s="10"/>
+      <c r="A39" s="14">
+        <v>37</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>229</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F39" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="G39" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I39" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J39" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="K39" s="10">
+        <v>1.41</v>
+      </c>
+      <c r="L39" s="1">
+        <v>1</v>
+      </c>
+      <c r="M39" s="8">
+        <f t="shared" si="0"/>
+        <v>1.41</v>
+      </c>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K40" s="10"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K41" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>